<commit_message>
Add Excel row index demo
</commit_message>
<xml_diff>
--- a/src/test/resources/templates/common-functions-complex.xlsx
+++ b/src/test/resources/templates/common-functions-complex.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\github-simter\simter-build\simter-jxls-ext\src\test\resources\templates\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="19830" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
@@ -17,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$3:$3</definedName>
   </definedNames>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="145621" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -32,7 +27,7 @@
     <author>RJ</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -43,11 +38,11 @@
             <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>jx:area(lastCell="F6")</t>
+          <t>jx:area(lastCell="G6")</t>
         </r>
       </text>
     </comment>
-    <comment ref="A4" authorId="0" shapeId="0">
+    <comment ref="A4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -58,7 +53,7 @@
             <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>jx:each(items="rows" var="r" lastCell="F4")</t>
+          <t>jx:each(items="rows" var="r" lastCell="G4")</t>
         </r>
       </text>
     </comment>
@@ -67,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Stage</t>
     <phoneticPr fontId="8" type="noConversion"/>
@@ -130,18 +125,30 @@
   </si>
   <si>
     <t>Custom Functions: fn.format, fn.toInt</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sn</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total:</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>$[ROW()-ROW(A3)]</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="176" formatCode="0_ "/>
     <numFmt numFmtId="177" formatCode="\$#,##0.00;\-\$#,##0.00"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -257,7 +264,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -310,6 +317,12 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -401,13 +414,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -444,13 +457,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -743,7 +756,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -754,7 +767,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozenSplit"/>
@@ -762,82 +775,99 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.25" style="1" customWidth="1"/>
-    <col min="2" max="2" width="45.75" style="1" customWidth="1"/>
-    <col min="3" max="3" width="56.625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.25" style="1" customWidth="1"/>
-    <col min="6" max="6" width="45" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="23.25" style="1" customWidth="1"/>
+    <col min="3" max="3" width="45.75" style="1" customWidth="1"/>
+    <col min="4" max="4" width="56.625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.25" style="1" customWidth="1"/>
+    <col min="7" max="7" width="45" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="5" customFormat="1" ht="38.25" customHeight="1">
+    <row r="1" spans="1:7" s="5" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="4"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="4"/>
     </row>
-    <row r="2" spans="1:6" s="6" customFormat="1" ht="24" customHeight="1">
+    <row r="2" spans="1:7" s="6" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="8" customFormat="1" ht="24" customHeight="1">
+    <row r="3" spans="1:7" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="C3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="D3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="E3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="F3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="G3" s="7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="9" customFormat="1" ht="24" customHeight="1">
+    <row r="4" spans="1:7" s="9" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="C4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="D4" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="E4" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="F4" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="G4" s="12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="9" customFormat="1" ht="12" customHeight="1">
+    <row r="5" spans="1:7" s="9" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="14"/>
-      <c r="B5" s="15"/>
+      <c r="B5" s="14"/>
       <c r="C5" s="15"/>
-      <c r="D5" s="16"/>
+      <c r="D5" s="15"/>
       <c r="E5" s="16"/>
       <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
     </row>
-    <row r="6" spans="1:6" s="9" customFormat="1" ht="24" customHeight="1">
+    <row r="6" spans="1:7" s="9" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>5</v>
       </c>
+      <c r="B6" s="10"/>
+      <c r="E6" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="19">
+        <f>SUM(F4)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:6" s="6" customFormat="1">
+    <row r="8" spans="1:7" s="6" customFormat="1" ht="14.25" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>15</v>
       </c>

</xml_diff>